<commit_message>
add data and fix graphic
</commit_message>
<xml_diff>
--- a/db/data.xlsx
+++ b/db/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\priso\OneDrive\Desktop\BAXI\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A34182-3B25-481A-B994-17F92AEBD49F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C62C72-0A30-48A2-8D33-71897F38D7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EAB160BA-2D0A-412B-88F5-F57B2DEE788C}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{EAB160BA-2D0A-412B-88F5-F57B2DEE788C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="107">
   <si>
     <t xml:space="preserve"> Accepted Baxi</t>
   </si>
@@ -66,9 +66,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>employee</t>
   </si>
   <si>
@@ -280,6 +277,84 @@
   </si>
   <si>
     <t>Nekonam</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Jamebozorg</t>
+  </si>
+  <si>
+    <t>Mobina</t>
+  </si>
+  <si>
+    <t>Rajabi</t>
+  </si>
+  <si>
+    <t>Hassan</t>
+  </si>
+  <si>
+    <t>Solymani</t>
+  </si>
+  <si>
+    <t>Matin</t>
+  </si>
+  <si>
+    <t>Movahidi</t>
+  </si>
+  <si>
+    <t>Kazem</t>
+  </si>
+  <si>
+    <t>Housiny</t>
+  </si>
+  <si>
+    <t>Rahele</t>
+  </si>
+  <si>
+    <t>Asadi</t>
+  </si>
+  <si>
+    <t>Taheri</t>
+  </si>
+  <si>
+    <t>Kokab</t>
+  </si>
+  <si>
+    <t>Ahmad</t>
+  </si>
+  <si>
+    <t>password(meli code)</t>
+  </si>
+  <si>
+    <t>Shakiri</t>
+  </si>
+  <si>
+    <t>Qorbanzade</t>
+  </si>
+  <si>
+    <t>Shayan</t>
+  </si>
+  <si>
+    <t>Abdolahy</t>
+  </si>
+  <si>
+    <t>Kiana</t>
+  </si>
+  <si>
+    <t>Iravani</t>
+  </si>
+  <si>
+    <t>Mahdi</t>
+  </si>
+  <si>
+    <t>Kushanmehr</t>
+  </si>
+  <si>
+    <t>Yalda</t>
+  </si>
+  <si>
+    <t>Tahbaz</t>
   </si>
 </sst>
 </file>
@@ -637,7 +712,7 @@
   <dimension ref="A1:F91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -647,7 +722,7 @@
     <col min="3" max="3" width="17.5546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.77734375" style="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -668,7 +743,7 @@
         <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -679,10 +754,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -693,10 +768,10 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -707,10 +782,10 @@
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -721,10 +796,10 @@
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -735,10 +810,10 @@
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -749,10 +824,10 @@
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -763,10 +838,10 @@
         <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -777,10 +852,10 @@
         <v>0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -791,10 +866,10 @@
         <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -805,10 +880,10 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -819,10 +894,10 @@
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -833,10 +908,10 @@
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -847,10 +922,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -861,10 +936,10 @@
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -875,10 +950,10 @@
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -889,10 +964,10 @@
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -903,10 +978,10 @@
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -917,10 +992,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -931,10 +1006,10 @@
         <v>2</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -945,10 +1020,10 @@
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -959,10 +1034,10 @@
         <v>2</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -973,10 +1048,10 @@
         <v>2</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -987,10 +1062,10 @@
         <v>2</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1001,10 +1076,10 @@
         <v>2</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1015,10 +1090,10 @@
         <v>2</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1029,10 +1104,10 @@
         <v>2</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1043,10 +1118,10 @@
         <v>2</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1057,10 +1132,10 @@
         <v>3</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1071,10 +1146,10 @@
         <v>3</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1085,10 +1160,10 @@
         <v>3</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1099,10 +1174,10 @@
         <v>3</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1113,10 +1188,10 @@
         <v>3</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1127,10 +1202,10 @@
         <v>3</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1141,10 +1216,10 @@
         <v>3</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1155,10 +1230,10 @@
         <v>3</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1169,56 +1244,137 @@
         <v>3</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>9220015041</v>
       </c>
+      <c r="B38" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>9220015042</v>
       </c>
+      <c r="B39" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>9220015043</v>
       </c>
+      <c r="B40" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>9220015044</v>
       </c>
+      <c r="B41" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>9220015045</v>
       </c>
+      <c r="B42" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>9220015046</v>
       </c>
+      <c r="B43" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>9220015047</v>
       </c>
+      <c r="B44" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>9220015048</v>
       </c>
+      <c r="B45" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>9220015049</v>
       </c>
+      <c r="B46" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
@@ -1405,7 +1561,19 @@
         <v>9220015091</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E83" s="1">
+        <v>12345</v>
+      </c>
+      <c r="F83" s="1">
+        <v>12345</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -1413,7 +1581,19 @@
         <v>9220015092</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E84" s="1">
+        <v>123456</v>
+      </c>
+      <c r="F84" s="1">
+        <v>123456</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -1421,7 +1601,19 @@
         <v>9220015093</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E85" s="1">
+        <v>1234567</v>
+      </c>
+      <c r="F85" s="1">
+        <v>1234567</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -1429,7 +1621,19 @@
         <v>9220015094</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E86" s="1">
+        <v>22334455</v>
+      </c>
+      <c r="F86" s="1">
+        <v>22334455</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -1437,7 +1641,19 @@
         <v>9220015095</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E87" s="1">
+        <v>11225522</v>
+      </c>
+      <c r="F87" s="1">
+        <v>11225522</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -1445,7 +1661,19 @@
         <v>9220015096</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E88" s="1">
+        <v>778842</v>
+      </c>
+      <c r="F88" s="1">
+        <v>778842</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -1456,16 +1684,16 @@
         <v>4</v>
       </c>
       <c r="C89" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D89" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="E89" s="1">
-        <v>987654321</v>
+        <v>987654331</v>
       </c>
       <c r="F89" s="1">
-        <v>9876</v>
+        <v>98766</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -1476,10 +1704,10 @@
         <v>4</v>
       </c>
       <c r="C90" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="E90" s="1">
         <v>123456789</v>
@@ -1496,16 +1724,16 @@
         <v>4</v>
       </c>
       <c r="C91" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="E91" s="1">
         <v>372365825</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>